<commit_message>
Committing minor changes to files within, and major changes to thesis document
</commit_message>
<xml_diff>
--- a/Charts/Classification Results.xlsx
+++ b/Charts/Classification Results.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomrichmond/ThesisWork/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomrichmond/ThesisWork/Charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674521F8-2612-894D-9D2B-2754C0B62ED6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{ACB0750A-BB72-F54F-8CBA-4466F9492257}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{ACB0750A-BB72-F54F-8CBA-4466F9492257}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$34:$C$40</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$D$34:$D$40</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$C$34:$C$40</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$D$34:$D$40</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="16">
   <si>
     <t>SVM</t>
   </si>
@@ -73,12 +68,18 @@
   <si>
     <t>J48</t>
   </si>
+  <si>
+    <t>Naïve Bayes</t>
+  </si>
+  <si>
+    <t>Logistic</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -211,7 +212,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ROC</c:v>
+                  <c:v>SVM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2758,6 +2759,735 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Classification</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Results</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Medieval</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Renaissance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Baroque</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Classical</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Romantic</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Modern</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.96399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.93300000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-30AE-3F48-BED5-D3921406D66C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Logistic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Medieval</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Renaissance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Baroque</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Classical</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Romantic</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Modern</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.98099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80800000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92100000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92700000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.88500000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-30AE-3F48-BED5-D3921406D66C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Naïve Bayes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Medieval</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Renaissance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Baroque</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Classical</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Romantic</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Modern</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.93799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.871</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.83799999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-30AE-3F48-BED5-D3921406D66C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jrip</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Medieval</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Renaissance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Baroque</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Classical</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Romantic</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Modern</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.70499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.874</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70399999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.83599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.77300000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-30AE-3F48-BED5-D3921406D66C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>J48</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Medieval</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Renaissance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Baroque</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Classical</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Romantic</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Modern</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.79800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.80400000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.74099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.753</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.753</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-30AE-3F48-BED5-D3921406D66C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="73108448"/>
+        <c:axId val="73110144"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="73108448"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73110144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="73110144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73108448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2958,6 +3688,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5473,20 +6243,525 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>780866</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>14633</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>399866</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>116233</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5513,16 +6788,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>652670</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>90833</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>271670</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>191697</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5549,16 +6824,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>487017</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>100956</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>106017</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>92</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5585,16 +6860,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>172028</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>2886</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>245651</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76509</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>628073</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>104486</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>701697</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>178109</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5621,15 +6896,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>389082</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>168213</xdr:colOff>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>34059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>833581</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600012</xdr:colOff>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>134506</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5650,6 +6925,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>297570</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>7416</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>757551</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>99375</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEAC7810-DD24-CF44-BEA3-58E04E951B59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5955,82 +7266,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95BB3B5-55BF-0D42-B2D9-E9ADC7E9FAEC}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2">
         <v>0.96399999999999997</v>
       </c>
+      <c r="E2">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="F2">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="G2">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="H2">
+        <v>0.79800000000000004</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3">
         <v>0.95799999999999996</v>
       </c>
+      <c r="E3">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="F3">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="G3">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="H3">
+        <v>0.77700000000000002</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4">
         <v>0.85399999999999998</v>
       </c>
+      <c r="E4">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="F4">
+        <v>0.73</v>
+      </c>
+      <c r="G4">
+        <v>0.73</v>
+      </c>
+      <c r="H4">
+        <v>0.68100000000000005</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5">
         <v>0.98799999999999999</v>
       </c>
+      <c r="E5">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="F5">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="G5">
+        <v>0.874</v>
+      </c>
+      <c r="H5">
+        <v>0.80400000000000005</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6">
         <v>0.83599999999999997</v>
       </c>
+      <c r="E6">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="G6">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="H6">
+        <v>0.74099999999999999</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7">
         <v>0.996</v>
       </c>
+      <c r="E7">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F7">
+        <v>0.871</v>
+      </c>
+      <c r="G7">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="H7">
+        <v>0.753</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8">
         <v>0.93300000000000005</v>
       </c>
+      <c r="E8">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="G8">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="H8">
+        <v>0.753</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -6041,7 +7445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="C10" t="s">
         <v>4</v>
       </c>
@@ -6049,7 +7453,7 @@
         <v>0.93799999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="C11" t="s">
         <v>9</v>
       </c>
@@ -6057,7 +7461,7 @@
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="C12" t="s">
         <v>8</v>
       </c>
@@ -6065,7 +7469,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="C13" t="s">
         <v>7</v>
       </c>
@@ -6073,7 +7477,7 @@
         <v>0.88900000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="C14" t="s">
         <v>6</v>
       </c>
@@ -6081,7 +7485,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="C15" t="s">
         <v>5</v>
       </c>
@@ -6089,7 +7493,7 @@
         <v>0.871</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="C16" t="s">
         <v>11</v>
       </c>
@@ -6097,7 +7501,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -6108,7 +7512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="C18" t="s">
         <v>4</v>
       </c>
@@ -6116,7 +7520,7 @@
         <v>0.98099999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="C19" t="s">
         <v>9</v>
       </c>
@@ -6124,7 +7528,7 @@
         <v>0.95099999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="C20" t="s">
         <v>8</v>
       </c>
@@ -6132,7 +7536,7 @@
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="C21" t="s">
         <v>7</v>
       </c>
@@ -6140,7 +7544,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="C22" t="s">
         <v>6</v>
       </c>
@@ -6148,7 +7552,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="C23" t="s">
         <v>5</v>
       </c>
@@ -6156,7 +7560,7 @@
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="C24" t="s">
         <v>11</v>
       </c>
@@ -6164,7 +7568,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -6175,7 +7579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="C26" t="s">
         <v>4</v>
       </c>
@@ -6183,7 +7587,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="C27" t="s">
         <v>9</v>
       </c>
@@ -6191,7 +7595,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="C28" t="s">
         <v>8</v>
       </c>
@@ -6199,7 +7603,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="C29" t="s">
         <v>7</v>
       </c>
@@ -6207,7 +7611,7 @@
         <v>0.874</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="C30" t="s">
         <v>6</v>
       </c>
@@ -6215,7 +7619,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="C31" t="s">
         <v>5</v>
       </c>
@@ -6223,7 +7627,7 @@
         <v>0.83599999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="C32" t="s">
         <v>11</v>
       </c>
@@ -6231,7 +7635,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -6242,7 +7646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="C34" t="s">
         <v>4</v>
       </c>
@@ -6250,7 +7654,7 @@
         <v>0.79800000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="C35" t="s">
         <v>9</v>
       </c>
@@ -6258,7 +7662,7 @@
         <v>0.77700000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="C36" t="s">
         <v>8</v>
       </c>
@@ -6266,7 +7670,7 @@
         <v>0.68100000000000005</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="C37" t="s">
         <v>7</v>
       </c>
@@ -6274,7 +7678,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="C38" t="s">
         <v>6</v>
       </c>
@@ -6282,7 +7686,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="C39" t="s">
         <v>5</v>
       </c>
@@ -6290,7 +7694,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="C40" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
committing any changes to presentations, as well as having a final copy of the thesis, and all its parts in isolation
</commit_message>
<xml_diff>
--- a/Charts/Classification Results.xlsx
+++ b/Charts/Classification Results.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomrichmond/ThesisWork/Charts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomrichmond/ThesisWork/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674521F8-2612-894D-9D2B-2754C0B62ED6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{ACB0750A-BB72-F54F-8CBA-4466F9492257}"/>
+    <workbookView minimized="1" xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{ACB0750A-BB72-F54F-8CBA-4466F9492257}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$34:$C$40</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$D$34:$D$40</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$C$34:$C$40</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$D$34:$D$40</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
   <si>
     <t>SVM</t>
   </si>
@@ -68,18 +73,12 @@
   <si>
     <t>J48</t>
   </si>
-  <si>
-    <t>Naïve Bayes</t>
-  </si>
-  <si>
-    <t>Logistic</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -212,7 +211,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SVM</c:v>
+                  <c:v>ROC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2759,735 +2758,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Classification</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Results</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SVM</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Medieval</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Renaissance</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Baroque</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Classical</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Romantic</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Modern</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Average</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.96399999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.95799999999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.85399999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.98799999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.83599999999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.996</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.93300000000000005</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-30AE-3F48-BED5-D3921406D66C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Logistic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Medieval</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Renaissance</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Baroque</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Classical</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Romantic</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Modern</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Average</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$2:$E$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.98099999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.95099999999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.80800000000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.92100000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.88500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.92700000000000005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.88500000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-30AE-3F48-BED5-D3921406D66C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Naïve Bayes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Medieval</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Renaissance</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Baroque</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Classical</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Romantic</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Modern</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Average</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$2:$F$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.93799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.93100000000000005</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.73</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.88900000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.85299999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.871</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.83799999999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-30AE-3F48-BED5-D3921406D66C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Jrip</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Medieval</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Renaissance</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Baroque</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Classical</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Romantic</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Modern</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Average</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$2:$G$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.70499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.84099999999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.73</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.874</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.70399999999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.83599999999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.77300000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-30AE-3F48-BED5-D3921406D66C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>J48</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Medieval</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Renaissance</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Baroque</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Classical</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Romantic</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Modern</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Average</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$2:$H$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.79800000000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.77700000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.68100000000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.80400000000000005</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.74099999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.753</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.753</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-30AE-3F48-BED5-D3921406D66C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="73108448"/>
-        <c:axId val="73110144"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="73108448"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="73110144"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="73110144"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="t"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="73108448"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3688,46 +2958,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6243,525 +5473,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>780866</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>14633</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>399866</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>116233</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6788,16 +5513,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>652670</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>90833</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>271670</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>191697</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6824,16 +5549,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>487017</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>100956</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>106017</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>92</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6860,16 +5585,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>245651</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>76509</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>172028</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>2886</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>701697</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>178109</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>628073</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>104486</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6896,15 +5621,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>168213</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>389082</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>34059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>600012</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>833581</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>134506</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6925,42 +5650,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>297570</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>7416</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>757551</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>99375</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEAC7810-DD24-CF44-BEA3-58E04E951B59}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7266,175 +5955,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95BB3B5-55BF-0D42-B2D9-E9ADC7E9FAEC}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection sqref="A1:D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
       <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2">
         <v>0.96399999999999997</v>
       </c>
-      <c r="E2">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="F2">
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="G2">
-        <v>0.70499999999999996</v>
-      </c>
-      <c r="H2">
-        <v>0.79800000000000004</v>
-      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3">
         <v>0.95799999999999996</v>
       </c>
-      <c r="E3">
-        <v>0.95099999999999996</v>
-      </c>
-      <c r="F3">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="G3">
-        <v>0.84099999999999997</v>
-      </c>
-      <c r="H3">
-        <v>0.77700000000000002</v>
-      </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4">
         <v>0.85399999999999998</v>
       </c>
-      <c r="E4">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="F4">
-        <v>0.73</v>
-      </c>
-      <c r="G4">
-        <v>0.73</v>
-      </c>
-      <c r="H4">
-        <v>0.68100000000000005</v>
-      </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5">
         <v>0.98799999999999999</v>
       </c>
-      <c r="E5">
-        <v>0.92100000000000004</v>
-      </c>
-      <c r="F5">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="G5">
-        <v>0.874</v>
-      </c>
-      <c r="H5">
-        <v>0.80400000000000005</v>
-      </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6">
         <v>0.83599999999999997</v>
       </c>
-      <c r="E6">
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="F6">
-        <v>0.85299999999999998</v>
-      </c>
-      <c r="G6">
-        <v>0.70399999999999996</v>
-      </c>
-      <c r="H6">
-        <v>0.74099999999999999</v>
-      </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7">
         <v>0.996</v>
       </c>
-      <c r="E7">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="F7">
-        <v>0.871</v>
-      </c>
-      <c r="G7">
-        <v>0.83599999999999997</v>
-      </c>
-      <c r="H7">
-        <v>0.753</v>
-      </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8">
         <v>0.93300000000000005</v>
       </c>
-      <c r="E8">
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="F8">
-        <v>0.83799999999999997</v>
-      </c>
-      <c r="G8">
-        <v>0.77300000000000002</v>
-      </c>
-      <c r="H8">
-        <v>0.753</v>
-      </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -7445,7 +6041,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>4</v>
       </c>
@@ -7453,7 +6049,7 @@
         <v>0.93799999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>9</v>
       </c>
@@ -7461,7 +6057,7 @@
         <v>0.93100000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>8</v>
       </c>
@@ -7469,7 +6065,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>7</v>
       </c>
@@ -7477,7 +6073,7 @@
         <v>0.88900000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>6</v>
       </c>
@@ -7485,7 +6081,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>5</v>
       </c>
@@ -7493,7 +6089,7 @@
         <v>0.871</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>11</v>
       </c>
@@ -7501,7 +6097,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -7512,7 +6108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>4</v>
       </c>
@@ -7520,7 +6116,7 @@
         <v>0.98099999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>9</v>
       </c>
@@ -7528,7 +6124,7 @@
         <v>0.95099999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>8</v>
       </c>
@@ -7536,7 +6132,7 @@
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>7</v>
       </c>
@@ -7544,7 +6140,7 @@
         <v>0.92100000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>6</v>
       </c>
@@ -7552,7 +6148,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>5</v>
       </c>
@@ -7560,7 +6156,7 @@
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>11</v>
       </c>
@@ -7568,7 +6164,7 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -7579,7 +6175,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>4</v>
       </c>
@@ -7587,7 +6183,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>9</v>
       </c>
@@ -7595,7 +6191,7 @@
         <v>0.84099999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>8</v>
       </c>
@@ -7603,7 +6199,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>7</v>
       </c>
@@ -7611,7 +6207,7 @@
         <v>0.874</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>6</v>
       </c>
@@ -7619,7 +6215,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>5</v>
       </c>
@@ -7627,7 +6223,7 @@
         <v>0.83599999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>11</v>
       </c>
@@ -7635,7 +6231,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -7646,7 +6242,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>4</v>
       </c>
@@ -7654,7 +6250,7 @@
         <v>0.79800000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
         <v>9</v>
       </c>
@@ -7662,7 +6258,7 @@
         <v>0.77700000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
         <v>8</v>
       </c>
@@ -7670,7 +6266,7 @@
         <v>0.68100000000000005</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
         <v>7</v>
       </c>
@@ -7678,7 +6274,7 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>6</v>
       </c>
@@ -7686,7 +6282,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>5</v>
       </c>
@@ -7694,7 +6290,7 @@
         <v>0.753</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>11</v>
       </c>

</xml_diff>